<commit_message>
Versao 7 com medida de impedancia
</commit_message>
<xml_diff>
--- a/Documentos/Simulação.xlsx
+++ b/Documentos/Simulação.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvio\TIE-Teste_01\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -156,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -216,11 +216,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,10 +280,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -283,20 +294,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +592,7 @@
   <dimension ref="A1:P179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,35 +611,35 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="F2" s="24" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="F2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>28</v>
@@ -649,7 +661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -677,7 +689,7 @@
         <v>70.980198019802074</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -705,7 +717,7 @@
         <v>74.643564356435675</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -733,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -760,8 +772,9 @@
       <c r="I7" s="15">
         <v>11.792079207920754</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="30"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -789,7 +802,7 @@
         <v>15.920792079207935</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -817,7 +830,7 @@
         <v>28.297029702970303</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -845,7 +858,7 @@
         <v>41.59405940594057</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -869,31 +882,31 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="21">
         <v>56.376237623762393</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="F13" s="22" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="F13" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12" t="s">
         <v>18</v>
@@ -915,7 +928,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>0</v>
       </c>
@@ -943,7 +956,7 @@
         <v>100.10891089108908</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>1</v>
       </c>
@@ -1149,18 +1162,18 @@
       <c r="I23" s="17"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="F24" s="22" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="F24" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -1415,18 +1428,18 @@
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="F35" s="24" t="s">
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="F35" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
@@ -1479,8 +1492,8 @@
         <v>0</v>
       </c>
       <c r="J37" s="2"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
@@ -1753,18 +1766,18 @@
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="F47" s="21" t="s">
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="F47" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
@@ -2013,18 +2026,18 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="F58" s="21" t="s">
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="F58" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
@@ -2279,18 +2292,18 @@
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="F69" s="21" t="s">
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="F69" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
@@ -2545,18 +2558,18 @@
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="21" t="s">
+      <c r="A80" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
-      <c r="F80" s="21" t="s">
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="F80" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G80" s="21"/>
-      <c r="H80" s="21"/>
-      <c r="I80" s="21"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="28"/>
+      <c r="I80" s="28"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
@@ -2875,18 +2888,18 @@
       <c r="J91" s="13"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A92" s="21" t="s">
+      <c r="A92" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
-      <c r="F92" s="21" t="s">
+      <c r="B92" s="28"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="F92" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G92" s="21"/>
-      <c r="H92" s="21"/>
-      <c r="I92" s="21"/>
+      <c r="G92" s="28"/>
+      <c r="H92" s="28"/>
+      <c r="I92" s="28"/>
       <c r="J92" s="2"/>
     </row>
     <row r="93" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3150,17 +3163,17 @@
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" s="24" t="s">
+      <c r="A103" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B103" s="25"/>
-      <c r="C103" s="25"/>
+      <c r="B103" s="23"/>
+      <c r="C103" s="23"/>
       <c r="D103" s="26"/>
-      <c r="F103" s="24" t="s">
+      <c r="F103" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G103" s="25"/>
-      <c r="H103" s="25"/>
+      <c r="G103" s="23"/>
+      <c r="H103" s="23"/>
       <c r="I103" s="26"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -3423,18 +3436,18 @@
       <c r="H113" s="8"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A114" s="21" t="s">
+      <c r="A114" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B114" s="21"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="21"/>
-      <c r="F114" s="21" t="s">
+      <c r="B114" s="28"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="F114" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G114" s="21"/>
-      <c r="H114" s="21"/>
-      <c r="I114" s="21"/>
+      <c r="G114" s="28"/>
+      <c r="H114" s="28"/>
+      <c r="I114" s="28"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
@@ -3696,18 +3709,18 @@
       <c r="H124" s="8"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A125" s="21" t="s">
+      <c r="A125" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B125" s="21"/>
-      <c r="C125" s="21"/>
-      <c r="D125" s="21"/>
-      <c r="F125" s="21" t="s">
+      <c r="B125" s="28"/>
+      <c r="C125" s="28"/>
+      <c r="D125" s="28"/>
+      <c r="F125" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G125" s="21"/>
-      <c r="H125" s="21"/>
-      <c r="I125" s="21"/>
+      <c r="G125" s="28"/>
+      <c r="H125" s="28"/>
+      <c r="I125" s="28"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
@@ -3983,18 +3996,18 @@
       <c r="I136" s="27"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="21" t="s">
+      <c r="A137" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B137" s="21"/>
-      <c r="C137" s="21"/>
-      <c r="D137" s="21"/>
-      <c r="F137" s="21" t="s">
+      <c r="B137" s="28"/>
+      <c r="C137" s="28"/>
+      <c r="D137" s="28"/>
+      <c r="F137" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G137" s="21"/>
-      <c r="H137" s="21"/>
-      <c r="I137" s="21"/>
+      <c r="G137" s="28"/>
+      <c r="H137" s="28"/>
+      <c r="I137" s="28"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
@@ -4243,17 +4256,17 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="24" t="s">
+      <c r="A148" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B148" s="25"/>
-      <c r="C148" s="25"/>
+      <c r="B148" s="23"/>
+      <c r="C148" s="23"/>
       <c r="D148" s="26"/>
-      <c r="F148" s="24" t="s">
+      <c r="F148" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G148" s="25"/>
-      <c r="H148" s="25"/>
+      <c r="G148" s="23"/>
+      <c r="H148" s="23"/>
       <c r="I148" s="26"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -4509,17 +4522,17 @@
       <c r="H158" s="8"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="24" t="s">
+      <c r="A159" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B159" s="25"/>
-      <c r="C159" s="25"/>
+      <c r="B159" s="23"/>
+      <c r="C159" s="23"/>
       <c r="D159" s="26"/>
-      <c r="F159" s="24" t="s">
+      <c r="F159" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G159" s="25"/>
-      <c r="H159" s="25"/>
+      <c r="G159" s="23"/>
+      <c r="H159" s="23"/>
       <c r="I159" s="26"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -4775,17 +4788,17 @@
       <c r="H169" s="8"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A170" s="24" t="s">
+      <c r="A170" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B170" s="25"/>
-      <c r="C170" s="25"/>
+      <c r="B170" s="23"/>
+      <c r="C170" s="23"/>
       <c r="D170" s="26"/>
-      <c r="F170" s="24" t="s">
+      <c r="F170" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G170" s="25"/>
-      <c r="H170" s="25"/>
+      <c r="G170" s="23"/>
+      <c r="H170" s="23"/>
       <c r="I170" s="26"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -5043,6 +5056,34 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A91:I91"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="A46:I46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="A114:D114"/>
+    <mergeCell ref="F114:I114"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="F125:I125"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="F137:I137"/>
+    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="F148:I148"/>
+    <mergeCell ref="A159:D159"/>
+    <mergeCell ref="F159:I159"/>
+    <mergeCell ref="A170:D170"/>
+    <mergeCell ref="F170:I170"/>
+    <mergeCell ref="A136:I136"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="F35:I35"/>
@@ -5051,34 +5092,6 @@
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A159:D159"/>
-    <mergeCell ref="F159:I159"/>
-    <mergeCell ref="A170:D170"/>
-    <mergeCell ref="F170:I170"/>
-    <mergeCell ref="A136:I136"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="F125:I125"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="F137:I137"/>
-    <mergeCell ref="A148:D148"/>
-    <mergeCell ref="F148:I148"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="F103:I103"/>
-    <mergeCell ref="A114:D114"/>
-    <mergeCell ref="F114:I114"/>
-    <mergeCell ref="A46:I46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="A91:I91"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="F69:I69"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5115,16 +5128,16 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="21"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="6"/>
       <c r="I2" s="9" t="s">
         <v>9</v>

</xml_diff>